<commit_message>
Cast Data for analysis updated
</commit_message>
<xml_diff>
--- a/Trial.xlsx
+++ b/Trial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tatai\Python files\Personal Projects Py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75170FC-1C7D-47A8-A4BC-3215D7A9E205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D18F26E-026C-4331-9EBA-D99EAA944F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="161">
   <si>
     <t>Popular Movies</t>
   </si>
@@ -76,6 +76,75 @@
     <t>dp ==1</t>
   </si>
   <si>
+    <t>The Proposal</t>
+  </si>
+  <si>
+    <t>2009</t>
+  </si>
+  <si>
+    <t>Baywatch</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>Central Intelligence</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>Red Notice</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>Jumanji: The Next Level</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>The Hitman's Bodyguard</t>
+  </si>
+  <si>
+    <t>6 Underground</t>
+  </si>
+  <si>
+    <t>Before We Go</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>Serena</t>
+  </si>
+  <si>
+    <t>47 Ronin</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>Fantastic Four</t>
+  </si>
+  <si>
+    <t>2005</t>
+  </si>
+  <si>
+    <t>Hot Pursuit</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>Ghost in the shell</t>
+  </si>
+  <si>
+    <t>Gemini Man</t>
+  </si>
+  <si>
     <t>Average/Good Movies</t>
   </si>
   <si>
@@ -88,42 +157,6 @@
     <t>Good</t>
   </si>
   <si>
-    <t>The Proposal</t>
-  </si>
-  <si>
-    <t>2009</t>
-  </si>
-  <si>
-    <t>Baywatch</t>
-  </si>
-  <si>
-    <t>2017</t>
-  </si>
-  <si>
-    <t>Central Intelligence</t>
-  </si>
-  <si>
-    <t>2016</t>
-  </si>
-  <si>
-    <t>Red Notice</t>
-  </si>
-  <si>
-    <t>2021</t>
-  </si>
-  <si>
-    <t>Jumanji: The Next Level</t>
-  </si>
-  <si>
-    <t>2019</t>
-  </si>
-  <si>
-    <t>The Hitman's Bodyguard</t>
-  </si>
-  <si>
-    <t>6 Underground</t>
-  </si>
-  <si>
     <t>The Killing of a Sacred Deer</t>
   </si>
   <si>
@@ -133,48 +166,15 @@
     <t>Logan Lucky</t>
   </si>
   <si>
+    <t>Loving</t>
+  </si>
+  <si>
+    <t>Bad Times at the El Royale</t>
+  </si>
+  <si>
     <t>2018</t>
   </si>
   <si>
-    <t>Loving</t>
-  </si>
-  <si>
-    <t>Bad Times at the El Royale</t>
-  </si>
-  <si>
-    <t>Before We Go</t>
-  </si>
-  <si>
-    <t>2014</t>
-  </si>
-  <si>
-    <t>Serena</t>
-  </si>
-  <si>
-    <t>47 Ronin</t>
-  </si>
-  <si>
-    <t>2013</t>
-  </si>
-  <si>
-    <t>Fantastic Four</t>
-  </si>
-  <si>
-    <t>2005</t>
-  </si>
-  <si>
-    <t>Hot Pursuit</t>
-  </si>
-  <si>
-    <t>2015</t>
-  </si>
-  <si>
-    <t>Ghost in the shell</t>
-  </si>
-  <si>
-    <t>Gemini Man</t>
-  </si>
-  <si>
     <t>Don't Look Up</t>
   </si>
   <si>
@@ -440,6 +440,69 @@
   </si>
   <si>
     <t>Roma</t>
+  </si>
+  <si>
+    <t>Spider-Man: Homecoming</t>
+  </si>
+  <si>
+    <t>Wind River</t>
+  </si>
+  <si>
+    <t>Beauty and the Beast</t>
+  </si>
+  <si>
+    <t>The Greatest Showman</t>
+  </si>
+  <si>
+    <t>Guardians of the Galaxy Vol. 2</t>
+  </si>
+  <si>
+    <t>Baby Driver</t>
+  </si>
+  <si>
+    <t>Darkest Hour</t>
+  </si>
+  <si>
+    <t>Wonder Woman</t>
+  </si>
+  <si>
+    <t>Lady Bird</t>
+  </si>
+  <si>
+    <t>John Wick: Chapter 2</t>
+  </si>
+  <si>
+    <t>The Shape of Water</t>
+  </si>
+  <si>
+    <t>It</t>
+  </si>
+  <si>
+    <t>Get Out</t>
+  </si>
+  <si>
+    <t>The Man Who Invented Christmas</t>
+  </si>
+  <si>
+    <t>Molly's Game</t>
+  </si>
+  <si>
+    <t>Phantom Thread</t>
+  </si>
+  <si>
+    <t>The Florida Project</t>
+  </si>
+  <si>
+    <t>Good Time</t>
+  </si>
+  <si>
+    <t>Shot Caller</t>
+  </si>
+  <si>
+    <t>Hostiles</t>
+  </si>
+  <si>
+    <t>Papillon</t>
   </si>
 </sst>
 </file>
@@ -783,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J125"/>
+  <dimension ref="A1:J146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M129" sqref="M129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -960,10 +1023,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1">
         <v>6.7</v>
@@ -990,10 +1053,10 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C17" s="1">
         <v>5.5</v>
@@ -1020,10 +1083,10 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C18" s="1">
         <v>6.3</v>
@@ -1050,10 +1113,10 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C19" s="1">
         <v>6.4</v>
@@ -1080,10 +1143,10 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C20" s="5">
         <v>6.7</v>
@@ -1110,10 +1173,10 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C21" s="6">
         <v>6.9</v>
@@ -1140,10 +1203,10 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C22" s="6">
         <v>6.1</v>
@@ -1170,10 +1233,10 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C23" s="1">
         <v>6.8</v>
@@ -1200,10 +1263,10 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C24" s="1">
         <v>5.4</v>
@@ -1230,10 +1293,10 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C25" s="1">
         <v>6.3</v>
@@ -1260,10 +1323,10 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C26" s="1">
         <v>5.7</v>
@@ -1290,10 +1353,10 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C27" s="1">
         <v>5.2</v>
@@ -1320,10 +1383,10 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C28" s="1">
         <v>6.3</v>
@@ -1350,7 +1413,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B29" s="1">
         <v>2019</v>
@@ -1413,7 +1476,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="D34" t="s">
         <v>1</v>
@@ -1427,16 +1490,16 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>5</v>
@@ -1456,10 +1519,10 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C37" s="1">
         <v>7</v>
@@ -1486,10 +1549,10 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C38" s="1">
         <v>7</v>
@@ -1516,10 +1579,10 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C39" s="1">
         <v>7</v>
@@ -1546,10 +1609,10 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C40" s="1">
         <v>7</v>
@@ -1576,10 +1639,10 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C41" s="1">
         <v>7.1</v>
@@ -1609,7 +1672,7 @@
         <v>51</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>52</v>
@@ -1620,7 +1683,7 @@
         <v>53</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>52</v>
@@ -1631,7 +1694,7 @@
         <v>54</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>55</v>
@@ -1642,7 +1705,7 @@
         <v>56</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>57</v>
@@ -1653,7 +1716,7 @@
         <v>58</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>59</v>
@@ -1664,7 +1727,7 @@
         <v>60</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>61</v>
@@ -1675,7 +1738,7 @@
         <v>62</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>61</v>
@@ -1686,7 +1749,7 @@
         <v>63</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>57</v>
@@ -1697,7 +1760,7 @@
         <v>64</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>61</v>
@@ -1708,7 +1771,7 @@
         <v>65</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>59</v>
@@ -1719,7 +1782,7 @@
         <v>66</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>61</v>
@@ -1730,7 +1793,7 @@
         <v>67</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>61</v>
@@ -1741,7 +1804,7 @@
         <v>68</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>69</v>
@@ -1752,7 +1815,7 @@
         <v>70</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>61</v>
@@ -1763,7 +1826,7 @@
         <v>71</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>69</v>
@@ -1774,7 +1837,7 @@
         <v>72</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>59</v>
@@ -1785,7 +1848,7 @@
         <v>73</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>69</v>
@@ -1796,7 +1859,7 @@
         <v>74</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>57</v>
@@ -1807,7 +1870,7 @@
         <v>75</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>76</v>
@@ -1818,7 +1881,7 @@
         <v>77</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>76</v>
@@ -1829,7 +1892,7 @@
         <v>78</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>59</v>
@@ -1840,7 +1903,7 @@
         <v>79</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>80</v>
@@ -1851,7 +1914,7 @@
         <v>81</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>80</v>
@@ -1862,7 +1925,7 @@
         <v>82</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>61</v>
@@ -1873,7 +1936,7 @@
         <v>13</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>61</v>
@@ -1884,7 +1947,7 @@
         <v>83</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>57</v>
@@ -1895,7 +1958,7 @@
         <v>84</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>76</v>
@@ -1928,7 +1991,7 @@
         <v>87</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>61</v>
@@ -1939,7 +2002,7 @@
         <v>88</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>61</v>
@@ -1950,7 +2013,7 @@
         <v>89</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>52</v>
@@ -1972,7 +2035,7 @@
         <v>91</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>76</v>
@@ -1983,7 +2046,7 @@
         <v>92</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>52</v>
@@ -1994,7 +2057,7 @@
         <v>93</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>61</v>
@@ -2005,7 +2068,7 @@
         <v>94</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>80</v>
@@ -2016,7 +2079,7 @@
         <v>95</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>55</v>
@@ -2027,7 +2090,7 @@
         <v>96</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>57</v>
@@ -2038,7 +2101,7 @@
         <v>97</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>59</v>
@@ -2049,7 +2112,7 @@
         <v>98</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>52</v>
@@ -2060,7 +2123,7 @@
         <v>99</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>69</v>
@@ -2071,7 +2134,7 @@
         <v>100</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>57</v>
@@ -2082,7 +2145,7 @@
         <v>101</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>52</v>
@@ -2093,7 +2156,7 @@
         <v>102</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>69</v>
@@ -2104,7 +2167,7 @@
         <v>103</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>52</v>
@@ -2115,7 +2178,7 @@
         <v>104</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>52</v>
@@ -2126,7 +2189,7 @@
         <v>105</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>57</v>
@@ -2137,7 +2200,7 @@
         <v>106</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>55</v>
@@ -2148,7 +2211,7 @@
         <v>107</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>52</v>
@@ -2159,7 +2222,7 @@
         <v>108</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>55</v>
@@ -2170,7 +2233,7 @@
         <v>109</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>76</v>
@@ -2181,7 +2244,7 @@
         <v>110</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>61</v>
@@ -2192,7 +2255,7 @@
         <v>111</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>55</v>
@@ -2203,7 +2266,7 @@
         <v>112</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>57</v>
@@ -2214,7 +2277,7 @@
         <v>113</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>52</v>
@@ -2236,7 +2299,7 @@
         <v>115</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>80</v>
@@ -2247,7 +2310,7 @@
         <v>116</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>80</v>
@@ -2258,7 +2321,7 @@
         <v>117</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>69</v>
@@ -2280,7 +2343,7 @@
         <v>119</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>69</v>
@@ -2291,7 +2354,7 @@
         <v>120</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>52</v>
@@ -2302,7 +2365,7 @@
         <v>121</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>55</v>
@@ -2313,7 +2376,7 @@
         <v>122</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>52</v>
@@ -2324,7 +2387,7 @@
         <v>123</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>69</v>
@@ -2346,7 +2409,7 @@
         <v>125</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>57</v>
@@ -2357,7 +2420,7 @@
         <v>126</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>55</v>
@@ -2365,10 +2428,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>76</v>
@@ -2390,7 +2453,7 @@
         <v>128</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>61</v>
@@ -2401,7 +2464,7 @@
         <v>129</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>76</v>
@@ -2412,7 +2475,7 @@
         <v>130</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>52</v>
@@ -2423,7 +2486,7 @@
         <v>131</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>69</v>
@@ -2434,7 +2497,7 @@
         <v>132</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>55</v>
@@ -2445,7 +2508,7 @@
         <v>133</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>55</v>
@@ -2456,7 +2519,7 @@
         <v>134</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>55</v>
@@ -2467,7 +2530,7 @@
         <v>135</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>61</v>
@@ -2478,7 +2541,7 @@
         <v>136</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>57</v>
@@ -2489,7 +2552,7 @@
         <v>137</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>76</v>
@@ -2500,7 +2563,7 @@
         <v>138</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>69</v>
@@ -2511,18 +2574,256 @@
         <v>139</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B125" s="1"/>
-      <c r="C125" s="1"/>
+      <c r="A125" t="s">
+        <v>140</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>141</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>142</v>
+      </c>
+      <c r="B127" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>143</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>144</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>145</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>146</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>147</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>45</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>148</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>149</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>150</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>151</v>
+      </c>
+      <c r="B137" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>152</v>
+      </c>
+      <c r="B138" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>153</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>154</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>155</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>156</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>157</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>158</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>159</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>160</v>
+      </c>
+      <c r="B146" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
All test Cases Applied & Working
</commit_message>
<xml_diff>
--- a/Trial.xlsx
+++ b/Trial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tatai\Python files\Personal Projects Py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC1408E-17A9-4CE8-85A2-7C16AA2D6037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6F4F88-A9D3-49AC-929E-228FE6BCF323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -433,73 +433,73 @@
     <t>Creed II</t>
   </si>
   <si>
+    <t>Roma</t>
+  </si>
+  <si>
+    <t>Spider-Man: Homecoming</t>
+  </si>
+  <si>
+    <t>Wind River</t>
+  </si>
+  <si>
+    <t>Beauty and the Beast</t>
+  </si>
+  <si>
+    <t>The Greatest Showman</t>
+  </si>
+  <si>
+    <t>Guardians of the Galaxy Vol. 2</t>
+  </si>
+  <si>
+    <t>Baby Driver</t>
+  </si>
+  <si>
+    <t>Darkest Hour</t>
+  </si>
+  <si>
+    <t>Wonder Woman</t>
+  </si>
+  <si>
+    <t>Lady Bird</t>
+  </si>
+  <si>
+    <t>John Wick: Chapter 2</t>
+  </si>
+  <si>
+    <t>The Shape of Water</t>
+  </si>
+  <si>
+    <t>It</t>
+  </si>
+  <si>
+    <t>Get Out</t>
+  </si>
+  <si>
+    <t>The Man Who Invented Christmas</t>
+  </si>
+  <si>
+    <t>Molly's Game</t>
+  </si>
+  <si>
+    <t>Phantom Thread</t>
+  </si>
+  <si>
+    <t>The Florida Project</t>
+  </si>
+  <si>
+    <t>Good Time</t>
+  </si>
+  <si>
+    <t>Shot Caller</t>
+  </si>
+  <si>
+    <t>Hostiles</t>
+  </si>
+  <si>
+    <t>Papillon</t>
+  </si>
+  <si>
     <t>Den skyldige</t>
-  </si>
-  <si>
-    <t>Roma</t>
-  </si>
-  <si>
-    <t>Spider-Man: Homecoming</t>
-  </si>
-  <si>
-    <t>Wind River</t>
-  </si>
-  <si>
-    <t>Beauty and the Beast</t>
-  </si>
-  <si>
-    <t>The Greatest Showman</t>
-  </si>
-  <si>
-    <t>Guardians of the Galaxy Vol. 2</t>
-  </si>
-  <si>
-    <t>Baby Driver</t>
-  </si>
-  <si>
-    <t>Darkest Hour</t>
-  </si>
-  <si>
-    <t>Wonder Woman</t>
-  </si>
-  <si>
-    <t>Lady Bird</t>
-  </si>
-  <si>
-    <t>John Wick: Chapter 2</t>
-  </si>
-  <si>
-    <t>The Shape of Water</t>
-  </si>
-  <si>
-    <t>It</t>
-  </si>
-  <si>
-    <t>Get Out</t>
-  </si>
-  <si>
-    <t>The Man Who Invented Christmas</t>
-  </si>
-  <si>
-    <t>Molly's Game</t>
-  </si>
-  <si>
-    <t>Phantom Thread</t>
-  </si>
-  <si>
-    <t>The Florida Project</t>
-  </si>
-  <si>
-    <t>Good Time</t>
-  </si>
-  <si>
-    <t>Shot Caller</t>
-  </si>
-  <si>
-    <t>Hostiles</t>
-  </si>
-  <si>
-    <t>Papillon</t>
   </si>
 </sst>
 </file>
@@ -843,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J145"/>
+  <dimension ref="A1:J151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1558,9 +1558,15 @@
       <c r="G37" s="1">
         <v>1</v>
       </c>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
+      <c r="H37" s="1">
+        <v>1</v>
+      </c>
+      <c r="I37" s="1">
+        <v>0</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
@@ -1584,9 +1590,15 @@
       <c r="G38" s="1">
         <v>0</v>
       </c>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
+      <c r="H38" s="1">
+        <v>0</v>
+      </c>
+      <c r="I38" s="1">
+        <v>1</v>
+      </c>
+      <c r="J38" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
@@ -1610,9 +1622,15 @@
       <c r="G39" s="1">
         <v>0</v>
       </c>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
+      <c r="H39" s="1">
+        <v>0</v>
+      </c>
+      <c r="I39" s="1">
+        <v>1</v>
+      </c>
+      <c r="J39" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
@@ -1636,9 +1654,15 @@
       <c r="G40" s="1">
         <v>0</v>
       </c>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
+      <c r="H40" s="1">
+        <v>1</v>
+      </c>
+      <c r="I40" s="1">
+        <v>0</v>
+      </c>
+      <c r="J40" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
@@ -1662,9 +1686,15 @@
       <c r="G41" s="1">
         <v>0</v>
       </c>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
+      <c r="H41" s="1">
+        <v>1</v>
+      </c>
+      <c r="I41" s="1">
+        <v>0</v>
+      </c>
+      <c r="J41" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
@@ -1688,6 +1718,15 @@
       <c r="G42" s="1">
         <v>1</v>
       </c>
+      <c r="H42" s="1">
+        <v>1</v>
+      </c>
+      <c r="I42" s="1">
+        <v>0</v>
+      </c>
+      <c r="J42" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
@@ -1711,6 +1750,15 @@
       <c r="G43" s="1">
         <v>1</v>
       </c>
+      <c r="H43" s="1">
+        <v>0</v>
+      </c>
+      <c r="I43" s="1">
+        <v>0</v>
+      </c>
+      <c r="J43" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
@@ -1734,6 +1782,15 @@
       <c r="G44" s="1">
         <v>1</v>
       </c>
+      <c r="H44" s="1">
+        <v>0</v>
+      </c>
+      <c r="I44" s="1">
+        <v>1</v>
+      </c>
+      <c r="J44" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
@@ -1757,6 +1814,15 @@
       <c r="G45" s="1">
         <v>0</v>
       </c>
+      <c r="H45" s="1">
+        <v>1</v>
+      </c>
+      <c r="I45" s="1">
+        <v>0</v>
+      </c>
+      <c r="J45" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
@@ -1780,6 +1846,15 @@
       <c r="G46" s="1">
         <v>0</v>
       </c>
+      <c r="H46" s="1">
+        <v>1</v>
+      </c>
+      <c r="I46" s="1">
+        <v>0</v>
+      </c>
+      <c r="J46" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
@@ -1803,6 +1878,15 @@
       <c r="G47" s="1">
         <v>0</v>
       </c>
+      <c r="H47" s="1">
+        <v>1</v>
+      </c>
+      <c r="I47" s="1">
+        <v>0</v>
+      </c>
+      <c r="J47" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
@@ -1826,8 +1910,17 @@
       <c r="G48" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H48" s="1">
+        <v>1</v>
+      </c>
+      <c r="I48" s="1">
+        <v>0</v>
+      </c>
+      <c r="J48" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -1849,8 +1942,17 @@
       <c r="G49" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H49" s="1">
+        <v>1</v>
+      </c>
+      <c r="I49" s="1">
+        <v>0</v>
+      </c>
+      <c r="J49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>64</v>
       </c>
@@ -1872,8 +1974,17 @@
       <c r="G50" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H50" s="1">
+        <v>1</v>
+      </c>
+      <c r="I50" s="1">
+        <v>0</v>
+      </c>
+      <c r="J50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>65</v>
       </c>
@@ -1895,8 +2006,17 @@
       <c r="G51" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H51" s="1">
+        <v>1</v>
+      </c>
+      <c r="I51" s="1">
+        <v>0</v>
+      </c>
+      <c r="J51" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>66</v>
       </c>
@@ -1918,8 +2038,17 @@
       <c r="G52" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H52" s="1">
+        <v>0</v>
+      </c>
+      <c r="I52" s="1">
+        <v>1</v>
+      </c>
+      <c r="J52" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>67</v>
       </c>
@@ -1941,8 +2070,17 @@
       <c r="G53" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H53" s="1">
+        <v>1</v>
+      </c>
+      <c r="I53" s="1">
+        <v>0</v>
+      </c>
+      <c r="J53" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>69</v>
       </c>
@@ -1964,8 +2102,17 @@
       <c r="G54" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H54" s="1">
+        <v>1</v>
+      </c>
+      <c r="I54" s="1">
+        <v>0</v>
+      </c>
+      <c r="J54" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>70</v>
       </c>
@@ -1987,8 +2134,17 @@
       <c r="G55" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H55" s="1">
+        <v>0</v>
+      </c>
+      <c r="I55" s="1">
+        <v>0</v>
+      </c>
+      <c r="J55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>71</v>
       </c>
@@ -2010,8 +2166,17 @@
       <c r="G56" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H56" s="1">
+        <v>0</v>
+      </c>
+      <c r="I56" s="1">
+        <v>1</v>
+      </c>
+      <c r="J56" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>72</v>
       </c>
@@ -2033,8 +2198,17 @@
       <c r="G57" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H57" s="1">
+        <v>1</v>
+      </c>
+      <c r="I57" s="1">
+        <v>0</v>
+      </c>
+      <c r="J57" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>73</v>
       </c>
@@ -2056,8 +2230,17 @@
       <c r="G58" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H58" s="1">
+        <v>1</v>
+      </c>
+      <c r="I58" s="1">
+        <v>0</v>
+      </c>
+      <c r="J58" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -2079,8 +2262,17 @@
       <c r="G59" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H59" s="1">
+        <v>0</v>
+      </c>
+      <c r="I59" s="1">
+        <v>0</v>
+      </c>
+      <c r="J59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>76</v>
       </c>
@@ -2102,8 +2294,17 @@
       <c r="G60" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H60" s="1">
+        <v>1</v>
+      </c>
+      <c r="I60" s="1">
+        <v>0</v>
+      </c>
+      <c r="J60" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>77</v>
       </c>
@@ -2125,8 +2326,17 @@
       <c r="G61" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H61" s="1">
+        <v>1</v>
+      </c>
+      <c r="I61" s="1">
+        <v>0</v>
+      </c>
+      <c r="J61" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>78</v>
       </c>
@@ -2148,8 +2358,17 @@
       <c r="G62" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H62" s="1">
+        <v>1</v>
+      </c>
+      <c r="I62" s="1">
+        <v>0</v>
+      </c>
+      <c r="J62" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>80</v>
       </c>
@@ -2171,8 +2390,17 @@
       <c r="G63" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H63" s="1">
+        <v>1</v>
+      </c>
+      <c r="I63" s="1">
+        <v>0</v>
+      </c>
+      <c r="J63" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>81</v>
       </c>
@@ -2194,8 +2422,17 @@
       <c r="G64" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H64" s="1">
+        <v>1</v>
+      </c>
+      <c r="I64" s="1">
+        <v>0</v>
+      </c>
+      <c r="J64" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>13</v>
       </c>
@@ -2217,8 +2454,17 @@
       <c r="G65" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H65" s="1">
+        <v>1</v>
+      </c>
+      <c r="I65" s="1">
+        <v>0</v>
+      </c>
+      <c r="J65" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>82</v>
       </c>
@@ -2240,8 +2486,17 @@
       <c r="G66" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H66" s="1">
+        <v>1</v>
+      </c>
+      <c r="I66" s="1">
+        <v>0</v>
+      </c>
+      <c r="J66" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>83</v>
       </c>
@@ -2263,8 +2518,17 @@
       <c r="G67" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H67" s="1">
+        <v>1</v>
+      </c>
+      <c r="I67" s="1">
+        <v>0</v>
+      </c>
+      <c r="J67" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>84</v>
       </c>
@@ -2286,8 +2550,17 @@
       <c r="G68" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H68" s="1">
+        <v>1</v>
+      </c>
+      <c r="I68" s="1">
+        <v>0</v>
+      </c>
+      <c r="J68" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>85</v>
       </c>
@@ -2309,8 +2582,17 @@
       <c r="G69" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H69" s="1">
+        <v>1</v>
+      </c>
+      <c r="I69" s="1">
+        <v>0</v>
+      </c>
+      <c r="J69" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>86</v>
       </c>
@@ -2332,8 +2614,17 @@
       <c r="G70" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H70" s="1">
+        <v>0</v>
+      </c>
+      <c r="I70" s="1">
+        <v>0</v>
+      </c>
+      <c r="J70" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>87</v>
       </c>
@@ -2355,8 +2646,17 @@
       <c r="G71" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H71" s="1">
+        <v>1</v>
+      </c>
+      <c r="I71" s="1">
+        <v>0</v>
+      </c>
+      <c r="J71" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>88</v>
       </c>
@@ -2378,8 +2678,17 @@
       <c r="G72" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H72" s="1">
+        <v>1</v>
+      </c>
+      <c r="I72" s="1">
+        <v>0</v>
+      </c>
+      <c r="J72" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>89</v>
       </c>
@@ -2401,8 +2710,17 @@
       <c r="G73" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H73" s="1">
+        <v>1</v>
+      </c>
+      <c r="I73" s="1">
+        <v>0</v>
+      </c>
+      <c r="J73" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>90</v>
       </c>
@@ -2424,8 +2742,17 @@
       <c r="G74" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H74" s="1">
+        <v>1</v>
+      </c>
+      <c r="I74" s="1">
+        <v>0</v>
+      </c>
+      <c r="J74" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>91</v>
       </c>
@@ -2447,8 +2774,17 @@
       <c r="G75" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H75" s="1">
+        <v>0</v>
+      </c>
+      <c r="I75" s="1">
+        <v>1</v>
+      </c>
+      <c r="J75" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>92</v>
       </c>
@@ -2470,8 +2806,17 @@
       <c r="G76" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H76" s="1">
+        <v>0</v>
+      </c>
+      <c r="I76" s="1">
+        <v>0</v>
+      </c>
+      <c r="J76" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>93</v>
       </c>
@@ -2493,8 +2838,17 @@
       <c r="G77" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H77" s="1">
+        <v>1</v>
+      </c>
+      <c r="I77" s="1">
+        <v>0</v>
+      </c>
+      <c r="J77" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>94</v>
       </c>
@@ -2516,8 +2870,17 @@
       <c r="G78" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H78" s="1">
+        <v>0</v>
+      </c>
+      <c r="I78" s="1">
+        <v>1</v>
+      </c>
+      <c r="J78" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>95</v>
       </c>
@@ -2539,8 +2902,17 @@
       <c r="G79" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H79" s="1">
+        <v>1</v>
+      </c>
+      <c r="I79" s="1">
+        <v>0</v>
+      </c>
+      <c r="J79" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>96</v>
       </c>
@@ -2562,8 +2934,17 @@
       <c r="G80" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H80" s="1">
+        <v>1</v>
+      </c>
+      <c r="I80" s="1">
+        <v>0</v>
+      </c>
+      <c r="J80" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>97</v>
       </c>
@@ -2585,8 +2966,17 @@
       <c r="G81" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H81" s="1">
+        <v>1</v>
+      </c>
+      <c r="I81" s="1">
+        <v>0</v>
+      </c>
+      <c r="J81" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>98</v>
       </c>
@@ -2608,8 +2998,17 @@
       <c r="G82" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H82" s="1">
+        <v>1</v>
+      </c>
+      <c r="I82" s="1">
+        <v>0</v>
+      </c>
+      <c r="J82" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>99</v>
       </c>
@@ -2631,8 +3030,17 @@
       <c r="G83" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H83" s="1">
+        <v>1</v>
+      </c>
+      <c r="I83" s="1">
+        <v>0</v>
+      </c>
+      <c r="J83" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>100</v>
       </c>
@@ -2654,8 +3062,17 @@
       <c r="G84" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H84" s="1">
+        <v>0</v>
+      </c>
+      <c r="I84" s="1">
+        <v>1</v>
+      </c>
+      <c r="J84" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>101</v>
       </c>
@@ -2677,8 +3094,17 @@
       <c r="G85" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H85" s="1">
+        <v>1</v>
+      </c>
+      <c r="I85" s="1">
+        <v>0</v>
+      </c>
+      <c r="J85" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>102</v>
       </c>
@@ -2700,8 +3126,17 @@
       <c r="G86" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H86" s="1">
+        <v>1</v>
+      </c>
+      <c r="I86" s="1">
+        <v>0</v>
+      </c>
+      <c r="J86" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>103</v>
       </c>
@@ -2723,8 +3158,17 @@
       <c r="G87" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H87" s="1">
+        <v>1</v>
+      </c>
+      <c r="I87" s="1">
+        <v>0</v>
+      </c>
+      <c r="J87" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>104</v>
       </c>
@@ -2746,8 +3190,17 @@
       <c r="G88" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H88" s="1">
+        <v>0</v>
+      </c>
+      <c r="I88" s="1">
+        <v>0</v>
+      </c>
+      <c r="J88" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>105</v>
       </c>
@@ -2769,8 +3222,17 @@
       <c r="G89" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H89" s="1">
+        <v>1</v>
+      </c>
+      <c r="I89" s="1">
+        <v>0</v>
+      </c>
+      <c r="J89" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>106</v>
       </c>
@@ -2792,8 +3254,17 @@
       <c r="G90" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H90" s="1">
+        <v>0</v>
+      </c>
+      <c r="I90" s="1">
+        <v>1</v>
+      </c>
+      <c r="J90" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>107</v>
       </c>
@@ -2815,8 +3286,17 @@
       <c r="G91" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H91" s="1">
+        <v>0</v>
+      </c>
+      <c r="I91" s="1">
+        <v>0</v>
+      </c>
+      <c r="J91" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>108</v>
       </c>
@@ -2838,8 +3318,17 @@
       <c r="G92" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H92" s="1">
+        <v>0</v>
+      </c>
+      <c r="I92" s="1">
+        <v>0</v>
+      </c>
+      <c r="J92" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>109</v>
       </c>
@@ -2861,8 +3350,17 @@
       <c r="G93" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H93" s="1">
+        <v>1</v>
+      </c>
+      <c r="I93" s="1">
+        <v>0</v>
+      </c>
+      <c r="J93" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>110</v>
       </c>
@@ -2884,8 +3382,17 @@
       <c r="G94" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H94" s="1">
+        <v>0</v>
+      </c>
+      <c r="I94" s="1">
+        <v>1</v>
+      </c>
+      <c r="J94" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>111</v>
       </c>
@@ -2907,8 +3414,17 @@
       <c r="G95" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H95" s="1">
+        <v>1</v>
+      </c>
+      <c r="I95" s="1">
+        <v>0</v>
+      </c>
+      <c r="J95" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>112</v>
       </c>
@@ -2930,8 +3446,17 @@
       <c r="G96" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H96" s="1">
+        <v>1</v>
+      </c>
+      <c r="I96" s="1">
+        <v>0</v>
+      </c>
+      <c r="J96" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>113</v>
       </c>
@@ -2953,8 +3478,17 @@
       <c r="G97" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H97" s="1">
+        <v>1</v>
+      </c>
+      <c r="I97" s="1">
+        <v>0</v>
+      </c>
+      <c r="J97" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>114</v>
       </c>
@@ -2976,8 +3510,17 @@
       <c r="G98" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H98" s="1">
+        <v>1</v>
+      </c>
+      <c r="I98" s="1">
+        <v>0</v>
+      </c>
+      <c r="J98" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>115</v>
       </c>
@@ -2999,8 +3542,17 @@
       <c r="G99" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H99" s="1">
+        <v>1</v>
+      </c>
+      <c r="I99" s="1">
+        <v>0</v>
+      </c>
+      <c r="J99" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>116</v>
       </c>
@@ -3022,8 +3574,17 @@
       <c r="G100" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H100" s="1">
+        <v>1</v>
+      </c>
+      <c r="I100" s="1">
+        <v>0</v>
+      </c>
+      <c r="J100" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>117</v>
       </c>
@@ -3045,8 +3606,17 @@
       <c r="G101" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H101" s="1">
+        <v>1</v>
+      </c>
+      <c r="I101" s="1">
+        <v>0</v>
+      </c>
+      <c r="J101" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>118</v>
       </c>
@@ -3068,8 +3638,17 @@
       <c r="G102" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H102" s="1">
+        <v>1</v>
+      </c>
+      <c r="I102" s="1">
+        <v>0</v>
+      </c>
+      <c r="J102" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>119</v>
       </c>
@@ -3091,8 +3670,17 @@
       <c r="G103" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H103" s="1">
+        <v>1</v>
+      </c>
+      <c r="I103" s="1">
+        <v>0</v>
+      </c>
+      <c r="J103" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>120</v>
       </c>
@@ -3114,8 +3702,17 @@
       <c r="G104" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H104" s="1">
+        <v>1</v>
+      </c>
+      <c r="I104" s="1">
+        <v>0</v>
+      </c>
+      <c r="J104" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>121</v>
       </c>
@@ -3137,8 +3734,17 @@
       <c r="G105" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H105" s="1">
+        <v>0</v>
+      </c>
+      <c r="I105" s="1">
+        <v>0</v>
+      </c>
+      <c r="J105" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>122</v>
       </c>
@@ -3160,8 +3766,17 @@
       <c r="G106" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H106" s="1">
+        <v>1</v>
+      </c>
+      <c r="I106" s="1">
+        <v>0</v>
+      </c>
+      <c r="J106" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>123</v>
       </c>
@@ -3183,8 +3798,17 @@
       <c r="G107" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H107" s="1">
+        <v>1</v>
+      </c>
+      <c r="I107" s="1">
+        <v>0</v>
+      </c>
+      <c r="J107" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>124</v>
       </c>
@@ -3206,8 +3830,17 @@
       <c r="G108" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H108" s="1">
+        <v>1</v>
+      </c>
+      <c r="I108" s="1">
+        <v>0</v>
+      </c>
+      <c r="J108" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>125</v>
       </c>
@@ -3229,8 +3862,17 @@
       <c r="G109" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H109" s="1">
+        <v>0</v>
+      </c>
+      <c r="I109" s="1">
+        <v>1</v>
+      </c>
+      <c r="J109" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>49</v>
       </c>
@@ -3252,8 +3894,17 @@
       <c r="G110" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H110" s="1">
+        <v>1</v>
+      </c>
+      <c r="I110" s="1">
+        <v>0</v>
+      </c>
+      <c r="J110" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>126</v>
       </c>
@@ -3275,8 +3926,17 @@
       <c r="G111" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H111" s="1">
+        <v>1</v>
+      </c>
+      <c r="I111" s="1">
+        <v>0</v>
+      </c>
+      <c r="J111" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>127</v>
       </c>
@@ -3298,8 +3958,17 @@
       <c r="G112" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H112" s="1">
+        <v>1</v>
+      </c>
+      <c r="I112" s="1">
+        <v>0</v>
+      </c>
+      <c r="J112" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>128</v>
       </c>
@@ -3321,8 +3990,17 @@
       <c r="G113" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H113" s="1">
+        <v>1</v>
+      </c>
+      <c r="I113" s="1">
+        <v>0</v>
+      </c>
+      <c r="J113" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>129</v>
       </c>
@@ -3344,8 +4022,17 @@
       <c r="G114" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H114" s="1">
+        <v>1</v>
+      </c>
+      <c r="I114" s="1">
+        <v>0</v>
+      </c>
+      <c r="J114" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>130</v>
       </c>
@@ -3367,8 +4054,17 @@
       <c r="G115" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H115" s="1">
+        <v>0</v>
+      </c>
+      <c r="I115" s="1">
+        <v>1</v>
+      </c>
+      <c r="J115" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>131</v>
       </c>
@@ -3390,8 +4086,17 @@
       <c r="G116" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H116" s="1">
+        <v>0</v>
+      </c>
+      <c r="I116" s="1">
+        <v>0</v>
+      </c>
+      <c r="J116" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>132</v>
       </c>
@@ -3413,8 +4118,17 @@
       <c r="G117" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H117" s="1">
+        <v>1</v>
+      </c>
+      <c r="I117" s="1">
+        <v>0</v>
+      </c>
+      <c r="J117" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>133</v>
       </c>
@@ -3436,8 +4150,17 @@
       <c r="G118" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H118" s="1">
+        <v>1</v>
+      </c>
+      <c r="I118" s="1">
+        <v>0</v>
+      </c>
+      <c r="J118" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>134</v>
       </c>
@@ -3459,8 +4182,17 @@
       <c r="G119" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H119" s="1">
+        <v>1</v>
+      </c>
+      <c r="I119" s="1">
+        <v>0</v>
+      </c>
+      <c r="J119" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>135</v>
       </c>
@@ -3482,8 +4214,17 @@
       <c r="G120" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H120" s="1">
+        <v>0</v>
+      </c>
+      <c r="I120" s="1">
+        <v>1</v>
+      </c>
+      <c r="J120" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>136</v>
       </c>
@@ -3505,8 +4246,17 @@
       <c r="G121" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H121" s="1">
+        <v>1</v>
+      </c>
+      <c r="I121" s="1">
+        <v>0</v>
+      </c>
+      <c r="J121" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>137</v>
       </c>
@@ -3514,7 +4264,7 @@
         <v>50</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="D122" s="1">
         <v>0</v>
@@ -3528,19 +4278,28 @@
       <c r="G122" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H122" s="1">
+        <v>1</v>
+      </c>
+      <c r="I122" s="1">
+        <v>0</v>
+      </c>
+      <c r="J122" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>138</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D123" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E123" s="1">
         <v>0</v>
@@ -3549,10 +4308,19 @@
         <v>0</v>
       </c>
       <c r="G123" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="H123" s="1">
+        <v>1</v>
+      </c>
+      <c r="I123" s="1">
+        <v>0</v>
+      </c>
+      <c r="J123" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>139</v>
       </c>
@@ -3560,10 +4328,10 @@
         <v>21</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="D124" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E124" s="1">
         <v>0</v>
@@ -3572,18 +4340,27 @@
         <v>0</v>
       </c>
       <c r="G124" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="H124" s="1">
+        <v>1</v>
+      </c>
+      <c r="I124" s="1">
+        <v>0</v>
+      </c>
+      <c r="J124" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>140</v>
       </c>
-      <c r="B125" s="1" t="s">
-        <v>21</v>
+      <c r="B125" s="1">
+        <v>2017</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D125" s="1">
         <v>1</v>
@@ -3592,36 +4369,54 @@
         <v>0</v>
       </c>
       <c r="F125" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G125" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H125" s="1">
+        <v>0</v>
+      </c>
+      <c r="I125" s="1">
+        <v>0</v>
+      </c>
+      <c r="J125" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>141</v>
       </c>
-      <c r="B126" s="1">
-        <v>2017</v>
+      <c r="B126" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="D126" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E126" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F126" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G126" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H126" s="1">
+        <v>1</v>
+      </c>
+      <c r="I126" s="1">
+        <v>0</v>
+      </c>
+      <c r="J126" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>142</v>
       </c>
@@ -3632,19 +4427,28 @@
         <v>57</v>
       </c>
       <c r="D127" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E127" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F127" s="1">
         <v>0</v>
       </c>
       <c r="G127" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="H127" s="1">
+        <v>1</v>
+      </c>
+      <c r="I127" s="1">
+        <v>0</v>
+      </c>
+      <c r="J127" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>143</v>
       </c>
@@ -3655,19 +4459,28 @@
         <v>57</v>
       </c>
       <c r="D128" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E128" s="1">
         <v>0</v>
       </c>
       <c r="F128" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G128" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="H128" s="1">
+        <v>1</v>
+      </c>
+      <c r="I128" s="1">
+        <v>0</v>
+      </c>
+      <c r="J128" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>144</v>
       </c>
@@ -3675,7 +4488,7 @@
         <v>21</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D129" s="1">
         <v>0</v>
@@ -3687,10 +4500,19 @@
         <v>1</v>
       </c>
       <c r="G129" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="H129" s="1">
+        <v>0</v>
+      </c>
+      <c r="I129" s="1">
+        <v>1</v>
+      </c>
+      <c r="J129" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>145</v>
       </c>
@@ -3701,65 +4523,92 @@
         <v>61</v>
       </c>
       <c r="D130" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E130" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F130" s="1">
         <v>1</v>
       </c>
       <c r="G130" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="H130" s="1">
+        <v>1</v>
+      </c>
+      <c r="I130" s="1">
+        <v>0</v>
+      </c>
+      <c r="J130" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>146</v>
+        <v>45</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D131" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E131" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F131" s="1">
         <v>1</v>
       </c>
       <c r="G131" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="H131" s="1">
+        <v>1</v>
+      </c>
+      <c r="I131" s="1">
+        <v>0</v>
+      </c>
+      <c r="J131" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>45</v>
+        <v>146</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D132" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E132" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F132" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G132" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="H132" s="1">
+        <v>1</v>
+      </c>
+      <c r="I132" s="1">
+        <v>0</v>
+      </c>
+      <c r="J132" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>147</v>
       </c>
@@ -3767,22 +4616,31 @@
         <v>21</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="D133" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E133" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F133" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G133" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H133" s="1">
+        <v>1</v>
+      </c>
+      <c r="I133" s="1">
+        <v>0</v>
+      </c>
+      <c r="J133" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>148</v>
       </c>
@@ -3790,7 +4648,7 @@
         <v>21</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D134" s="1">
         <v>0</v>
@@ -3799,18 +4657,27 @@
         <v>2</v>
       </c>
       <c r="F134" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G134" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H134" s="1">
+        <v>0</v>
+      </c>
+      <c r="I134" s="1">
+        <v>1</v>
+      </c>
+      <c r="J134" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>149</v>
       </c>
-      <c r="B135" s="1" t="s">
-        <v>21</v>
+      <c r="B135" s="1">
+        <v>2017</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>52</v>
@@ -3819,16 +4686,25 @@
         <v>0</v>
       </c>
       <c r="E135" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F135" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G135" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="H135" s="1">
+        <v>0</v>
+      </c>
+      <c r="I135" s="1">
+        <v>1</v>
+      </c>
+      <c r="J135" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>150</v>
       </c>
@@ -3836,45 +4712,63 @@
         <v>2017</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="D136" s="1">
         <v>0</v>
       </c>
       <c r="E136" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F136" s="1">
         <v>1</v>
       </c>
       <c r="G136" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="H136" s="1">
+        <v>1</v>
+      </c>
+      <c r="I136" s="1">
+        <v>0</v>
+      </c>
+      <c r="J136" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>151</v>
       </c>
-      <c r="B137" s="1">
-        <v>2017</v>
+      <c r="B137" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="D137" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E137" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F137" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G137" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="H137" s="1">
+        <v>0</v>
+      </c>
+      <c r="I137" s="1">
+        <v>1</v>
+      </c>
+      <c r="J137" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>152</v>
       </c>
@@ -3882,10 +4776,10 @@
         <v>21</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D138" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E138" s="1">
         <v>0</v>
@@ -3894,10 +4788,19 @@
         <v>0</v>
       </c>
       <c r="G138" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="H138" s="1">
+        <v>1</v>
+      </c>
+      <c r="I138" s="1">
+        <v>0</v>
+      </c>
+      <c r="J138" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>153</v>
       </c>
@@ -3905,22 +4808,31 @@
         <v>21</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="D139" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E139" s="1">
         <v>0</v>
       </c>
       <c r="F139" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G139" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H139" s="1">
+        <v>1</v>
+      </c>
+      <c r="I139" s="1">
+        <v>0</v>
+      </c>
+      <c r="J139" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>154</v>
       </c>
@@ -3928,10 +4840,10 @@
         <v>21</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D140" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E140" s="1">
         <v>0</v>
@@ -3942,8 +4854,17 @@
       <c r="G140" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H140" s="1">
+        <v>1</v>
+      </c>
+      <c r="I140" s="1">
+        <v>0</v>
+      </c>
+      <c r="J140" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>155</v>
       </c>
@@ -3951,22 +4872,31 @@
         <v>21</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D141" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E141" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F141" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G141" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H141" s="1">
+        <v>0</v>
+      </c>
+      <c r="I141" s="1">
+        <v>0</v>
+      </c>
+      <c r="J141" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>156</v>
       </c>
@@ -3974,22 +4904,31 @@
         <v>21</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D142" s="1">
         <v>0</v>
       </c>
       <c r="E142" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F142" s="1">
         <v>0</v>
       </c>
       <c r="G142" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="H142" s="1">
+        <v>1</v>
+      </c>
+      <c r="I142" s="1">
+        <v>0</v>
+      </c>
+      <c r="J142" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>157</v>
       </c>
@@ -3997,27 +4936,36 @@
         <v>21</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D143" s="1">
         <v>0</v>
       </c>
       <c r="E143" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F143" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G143" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="H143" s="1">
+        <v>1</v>
+      </c>
+      <c r="I143" s="1">
+        <v>0</v>
+      </c>
+      <c r="J143" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>158</v>
       </c>
-      <c r="B144" s="1" t="s">
-        <v>21</v>
+      <c r="B144" s="1">
+        <v>2017</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>59</v>
@@ -4026,36 +4974,54 @@
         <v>0</v>
       </c>
       <c r="E144" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F144" s="1">
         <v>1</v>
       </c>
       <c r="G144" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A145" t="s">
+        <v>1</v>
+      </c>
+      <c r="H144" s="1">
+        <v>1</v>
+      </c>
+      <c r="I144" s="1">
+        <v>0</v>
+      </c>
+      <c r="J144" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
         <v>159</v>
       </c>
-      <c r="B145" s="1">
-        <v>2017</v>
-      </c>
-      <c r="C145" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D145" s="1">
-        <v>0</v>
-      </c>
-      <c r="E145" s="1">
-        <v>0</v>
-      </c>
-      <c r="F145" s="1">
-        <v>1</v>
-      </c>
-      <c r="G145" s="1">
-        <v>1</v>
+      <c r="B151" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D151" s="1">
+        <v>0</v>
+      </c>
+      <c r="E151" s="1">
+        <v>0</v>
+      </c>
+      <c r="F151" s="1">
+        <v>0</v>
+      </c>
+      <c r="G151" s="1">
+        <v>1</v>
+      </c>
+      <c r="H151" s="1">
+        <v>0</v>
+      </c>
+      <c r="I151" s="1">
+        <v>0</v>
+      </c>
+      <c r="J151" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>